<commit_message>
Removed remaining embargoed files to prepare OLRs for test ingest
</commit_message>
<xml_diff>
--- a/datamares/OLR/OLR_datamares_kelp.xlsx
+++ b/datamares/OLR/OLR_datamares_kelp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="21600" windowHeight="10545"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="21600" windowHeight="10545" tabRatio="511"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="639">
   <si>
     <t>text</t>
   </si>
@@ -1899,9 +1899,6 @@
   </si>
   <si>
     <t>Giron-Nava, Alfredo</t>
-  </si>
-  <si>
-    <t>k_po_kelp.xlsx</t>
   </si>
   <si>
     <t>Counting fish in the kelp forests of Baja California</t>
@@ -3099,7 +3096,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="R1" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3206,15 +3203,9 @@
       <c r="B2" s="17" t="s">
         <v>485</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>625</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>403</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>473</v>
-      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="17" t="s">
         <v>358</v>
       </c>
@@ -3222,10 +3213,10 @@
         <v>433</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>625</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>626</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>627</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>624</v>
@@ -3237,40 +3228,40 @@
         <v>623</v>
       </c>
       <c r="M2" s="17" t="s">
+        <v>627</v>
+      </c>
+      <c r="N2" s="17" t="s">
         <v>628</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="O2" s="17" t="s">
         <v>629</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="P2" s="21" t="s">
+        <v>636</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>631</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>635</v>
+      </c>
+      <c r="T2" s="17" t="s">
         <v>630</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="U2" s="17" t="s">
+        <v>638</v>
+      </c>
+      <c r="V2" s="17" t="s">
         <v>637</v>
       </c>
-      <c r="Q2" s="17" t="s">
+      <c r="W2" s="19" t="s">
+        <v>633</v>
+      </c>
+      <c r="X2" s="19" t="s">
         <v>632</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>636</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>631</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>639</v>
-      </c>
-      <c r="V2" s="17" t="s">
-        <v>638</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>634</v>
-      </c>
-      <c r="X2" s="19" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>